<commit_message>
Update Tachometer 2021-01-05 V1.xlsx
</commit_message>
<xml_diff>
--- a/test results/Tachometer 2021-01-05 V1.xlsx
+++ b/test results/Tachometer 2021-01-05 V1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL E5440 WIN10\Desktop\ME 481 Programs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL E5440 WIN10\Desktop\ME 481 Programs\test results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BD86AF-141E-46EE-8AEF-F897DEA4272D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C263EFF-2316-47C1-A4DB-130FC1013D39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D06F39D2-3E3A-4ABB-8858-BCE55410CC21}"/>
   </bookViews>
@@ -248,6 +248,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Motor Speed vs</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> Analog</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Pin Output</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1796,6 +1834,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Analog</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Pin Output</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1858,6 +1956,74 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Speed</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> (rpm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.3888888888888888E-2"/>
+              <c:y val="0.35319845435987168"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2848,7 +3014,7 @@
   <dimension ref="A1:G227"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>